<commit_message>
optimize SWI and SWI+C of MM
</commit_message>
<xml_diff>
--- a/MM/MM_data.xlsx
+++ b/MM/MM_data.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="MM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="200">
   <si>
     <t>ALUTs</t>
   </si>
@@ -562,6 +559,164 @@
     <t>3. SWI+Channel</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>basic_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pb_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use private memory for tB[1024*1024]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ul4_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ul8_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ul16_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ul32_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11 / 1,518 ( &lt; 1 % )</t>
+  </si>
+  <si>
+    <t>2,417 / 2,713 ( 89 % )</t>
+  </si>
+  <si>
+    <t>51,245 / 427,200 ( 12 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 / 1,518 ( &lt; 1 % )</t>
+  </si>
+  <si>
+    <t>3,781,136 / 55,562,240 ( 7 % )</t>
+  </si>
+  <si>
+    <t>385 / 2,713 ( 14 % )</t>
+  </si>
+  <si>
+    <t>14 / 1,518 ( &lt; 1 % )</t>
+  </si>
+  <si>
+    <t>4,111,056 / 55,562,240 ( 7 % )</t>
+  </si>
+  <si>
+    <t>420 / 2,713 ( 15 % )</t>
+  </si>
+  <si>
+    <t>22 / 1,518 ( 1 % )</t>
+  </si>
+  <si>
+    <t>4,780,816 / 55,562,240 ( 9 % )</t>
+  </si>
+  <si>
+    <t>493 / 2,713 ( 18 % )</t>
+  </si>
+  <si>
+    <t>38 / 1,518 ( 3 % )</t>
+  </si>
+  <si>
+    <t>7,726,224 / 55,562,240 ( 14 % )</t>
+  </si>
+  <si>
+    <t>715 / 2,713 ( 26 % )</t>
+  </si>
+  <si>
+    <t>47,126 / 427,200 ( 11 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>47,963 / 427,200 ( 11 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>37,079,056 / 55,562,240 ( 67 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>54,816 / 427,200 ( 13 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>63,805 / 427,200 ( 15 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>91,165 / 427,200 ( 21 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1_ul4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1_ul8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1_ul16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1-1_ul32</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>48,234 / 427,200 ( 11 % )</t>
+  </si>
+  <si>
+    <t>50,718 / 427,200 ( 12 % )</t>
+  </si>
+  <si>
+    <t>3,013,392 / 55,562,240 ( 5 % )</t>
+  </si>
+  <si>
+    <t>351 / 2,713 ( 13 % )</t>
+  </si>
+  <si>
+    <t>53,112 / 427,200 ( 12 % )</t>
+  </si>
+  <si>
+    <t>3,195,984 / 55,562,240 ( 6 % )</t>
+  </si>
+  <si>
+    <t>381 / 2,713 ( 14 % )</t>
+  </si>
+  <si>
+    <t>58,437 / 427,200 ( 14 % )</t>
+  </si>
+  <si>
+    <t>3,578,128 / 55,562,240 ( 6 % )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>442 / 2,713 ( 16 % )</t>
+  </si>
+  <si>
+    <t>74,269 / 427,200 ( 17 % )</t>
+  </si>
+  <si>
+    <t>5,222,288 / 55,562,240 ( 9 % )</t>
+  </si>
+  <si>
+    <t>575 / 2,713 ( 21 % )</t>
+  </si>
 </sst>
 </file>
 
@@ -571,7 +726,7 @@
     <numFmt numFmtId="176" formatCode="0.000_);[Red]\(0.000\)"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,6 +776,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -680,7 +842,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,6 +919,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,810 +958,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="summary"/>
-      <sheetName val="configurations"/>
-      <sheetName val="memory_bandwidth"/>
-      <sheetName val="KM"/>
-      <sheetName val="Kmeans"/>
-      <sheetName val="BFS"/>
-      <sheetName val="RSCD"/>
-      <sheetName val="TQH"/>
-      <sheetName val="HSTI"/>
-      <sheetName val="BS"/>
-      <sheetName val="SC"/>
-      <sheetName val="PAD"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="cedd"/>
-      <sheetName val="MM"/>
-      <sheetName val="MS"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
-        <row r="101">
-          <cell r="C101" t="str">
-            <v>float16</v>
-          </cell>
-          <cell r="D101" t="str">
-            <v>float</v>
-          </cell>
-          <cell r="E101" t="str">
-            <v>double</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="B102" t="str">
-            <v>Baseline</v>
-          </cell>
-          <cell r="C102">
-            <v>0.56247424810895252</v>
-          </cell>
-          <cell r="D102">
-            <v>0.56250923989034196</v>
-          </cell>
-          <cell r="E102">
-            <v>0.52492506164097108</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="B103" t="str">
-            <v>SIMD4</v>
-          </cell>
-          <cell r="C103">
-            <v>2.0957725579062219</v>
-          </cell>
-          <cell r="D103">
-            <v>2.1998375846777458</v>
-          </cell>
-          <cell r="E103">
-            <v>1.8233851456023396</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="B104" t="str">
-            <v>UL16</v>
-          </cell>
-          <cell r="C104">
-            <v>8.5501933015344687</v>
-          </cell>
-          <cell r="D104">
-            <v>8.2323067309922351</v>
-          </cell>
-          <cell r="E104">
-            <v>8.6774729470902461</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="B105" t="str">
-            <v>UL64</v>
-          </cell>
-          <cell r="C105">
-            <v>32.80504185634414</v>
-          </cell>
-          <cell r="D105">
-            <v>34.254781748721918</v>
-          </cell>
-          <cell r="E105">
-            <v>32.410200046785747</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="B106" t="str">
-            <v>UL64 + SIMD2</v>
-          </cell>
-          <cell r="C106">
-            <v>62.861765997306954</v>
-          </cell>
-          <cell r="D106">
-            <v>70.258417169684776</v>
-          </cell>
-          <cell r="E106">
-            <v>68.598743012298357</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="B107" t="str">
-            <v>UL64 + SIMD4</v>
-          </cell>
-          <cell r="C107">
-            <v>132.74919020832047</v>
-          </cell>
-          <cell r="D107">
-            <v>125.20310459421641</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="B108" t="str">
-            <v>UL64 + SIMD8</v>
-          </cell>
-          <cell r="C108">
-            <v>254.54674924435488</v>
-          </cell>
-          <cell r="D108">
-            <v>252.98741238145729</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="B109" t="str">
-            <v>UL64 + SIMD16</v>
-          </cell>
-          <cell r="D109">
-            <v>398.34606751994068</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="B110" t="str">
-            <v>UL64+SIMD2+CU3</v>
-          </cell>
-          <cell r="C110">
-            <v>195.55467376952146</v>
-          </cell>
-          <cell r="D110">
-            <v>189.13895103047386</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="B111" t="str">
-            <v>UL64+SIMD2 +CU4</v>
-          </cell>
-          <cell r="C111">
-            <v>233.84152556214951</v>
-          </cell>
-          <cell r="D111">
-            <v>242.81814224332885</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="B112" t="str">
-            <v>UL64+SIMD4+CU3</v>
-          </cell>
-          <cell r="C112">
-            <v>348.25000405416364</v>
-          </cell>
-          <cell r="D112">
-            <v>364.7220872961957</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="B113" t="str">
-            <v>UL64+SIMD8+CU2</v>
-          </cell>
-          <cell r="D113">
-            <v>470.88776449950666</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="C139" t="str">
-            <v>float16</v>
-          </cell>
-          <cell r="D139" t="str">
-            <v>float</v>
-          </cell>
-          <cell r="E139" t="str">
-            <v>double</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="B140" t="str">
-            <v>Baseline</v>
-          </cell>
-          <cell r="C140">
-            <v>50149</v>
-          </cell>
-          <cell r="D140">
-            <v>48944</v>
-          </cell>
-          <cell r="E140">
-            <v>52129</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="B141" t="str">
-            <v>SIMD4</v>
-          </cell>
-          <cell r="C141">
-            <v>55153</v>
-          </cell>
-          <cell r="D141">
-            <v>54947</v>
-          </cell>
-          <cell r="E141">
-            <v>66038</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="B142" t="str">
-            <v>UL16</v>
-          </cell>
-          <cell r="C142">
-            <v>54041</v>
-          </cell>
-          <cell r="D142">
-            <v>49979</v>
-          </cell>
-          <cell r="E142">
-            <v>79076</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="B143" t="str">
-            <v>UL64</v>
-          </cell>
-          <cell r="C143">
-            <v>64184</v>
-          </cell>
-          <cell r="D143">
-            <v>55483</v>
-          </cell>
-          <cell r="E143">
-            <v>170741</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="B144" t="str">
-            <v>UL64 + SIMD2</v>
-          </cell>
-          <cell r="C144">
-            <v>81248</v>
-          </cell>
-          <cell r="D144">
-            <v>60939</v>
-          </cell>
-          <cell r="E144">
-            <v>288501</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="B145" t="str">
-            <v>UL64 + SIMD4</v>
-          </cell>
-          <cell r="C145">
-            <v>114971</v>
-          </cell>
-          <cell r="D145">
-            <v>70694</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="B146" t="str">
-            <v>UL64 + SIMD8</v>
-          </cell>
-          <cell r="C146">
-            <v>180873</v>
-          </cell>
-          <cell r="D146">
-            <v>91744</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="B147" t="str">
-            <v>UL64 + SIMD16</v>
-          </cell>
-          <cell r="D147">
-            <v>132046</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="B148" t="str">
-            <v>UL64+SIMD2+CU3</v>
-          </cell>
-          <cell r="C148">
-            <v>157733</v>
-          </cell>
-          <cell r="D148">
-            <v>98272</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="B149" t="str">
-            <v>UL64+SIMD2 +CU4</v>
-          </cell>
-          <cell r="C149">
-            <v>196497</v>
-          </cell>
-          <cell r="D149">
-            <v>118059</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="B150" t="str">
-            <v>UL64+SIMD4+CU3</v>
-          </cell>
-          <cell r="C150">
-            <v>258013</v>
-          </cell>
-          <cell r="D150">
-            <v>127460</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="B151" t="str">
-            <v>UL64+SIMD8+CU2</v>
-          </cell>
-          <cell r="D151">
-            <v>139493</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="C156" t="str">
-            <v>float16</v>
-          </cell>
-          <cell r="D156" t="str">
-            <v>float</v>
-          </cell>
-          <cell r="E156" t="str">
-            <v>double</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="B157" t="str">
-            <v>Baseline</v>
-          </cell>
-          <cell r="C157">
-            <v>9</v>
-          </cell>
-          <cell r="D157">
-            <v>9</v>
-          </cell>
-          <cell r="E157">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="B158" t="str">
-            <v>SIMD4</v>
-          </cell>
-          <cell r="C158">
-            <v>12</v>
-          </cell>
-          <cell r="D158">
-            <v>12</v>
-          </cell>
-          <cell r="E158">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="B159" t="str">
-            <v>UL16</v>
-          </cell>
-          <cell r="C159">
-            <v>24</v>
-          </cell>
-          <cell r="D159">
-            <v>24</v>
-          </cell>
-          <cell r="E159">
-            <v>72</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="B160" t="str">
-            <v>UL64</v>
-          </cell>
-          <cell r="C160">
-            <v>72</v>
-          </cell>
-          <cell r="D160">
-            <v>72</v>
-          </cell>
-          <cell r="E160">
-            <v>264</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="B161" t="str">
-            <v>UL64 + SIMD2</v>
-          </cell>
-          <cell r="C161">
-            <v>136</v>
-          </cell>
-          <cell r="D161">
-            <v>136</v>
-          </cell>
-          <cell r="E161">
-            <v>520</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="B162" t="str">
-            <v>UL64 + SIMD4</v>
-          </cell>
-          <cell r="C162">
-            <v>264</v>
-          </cell>
-          <cell r="D162">
-            <v>264</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="B163" t="str">
-            <v>UL64 + SIMD8</v>
-          </cell>
-          <cell r="C163">
-            <v>520</v>
-          </cell>
-          <cell r="D163">
-            <v>520</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="B164" t="str">
-            <v>UL64 + SIMD16</v>
-          </cell>
-          <cell r="D164">
-            <v>1032</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="B165" t="str">
-            <v>UL64+SIMD2+CU3</v>
-          </cell>
-          <cell r="C165">
-            <v>408</v>
-          </cell>
-          <cell r="D165">
-            <v>408</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="B166" t="str">
-            <v>UL64+SIMD2 +CU4</v>
-          </cell>
-          <cell r="C166">
-            <v>544</v>
-          </cell>
-          <cell r="D166">
-            <v>544</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="B167" t="str">
-            <v>UL64+SIMD4+CU3</v>
-          </cell>
-          <cell r="C167">
-            <v>792</v>
-          </cell>
-          <cell r="D167">
-            <v>792</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="B168" t="str">
-            <v>UL64+SIMD8+CU2</v>
-          </cell>
-          <cell r="D168">
-            <v>1040</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="C173" t="str">
-            <v>float16</v>
-          </cell>
-          <cell r="D173" t="str">
-            <v>float</v>
-          </cell>
-          <cell r="E173" t="str">
-            <v>double</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="B174" t="str">
-            <v>Baseline</v>
-          </cell>
-          <cell r="C174">
-            <v>10010128</v>
-          </cell>
-          <cell r="D174">
-            <v>10898448</v>
-          </cell>
-          <cell r="E174">
-            <v>13165200</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="B175" t="str">
-            <v>SIMD4</v>
-          </cell>
-          <cell r="C175">
-            <v>6123536</v>
-          </cell>
-          <cell r="D175">
-            <v>7194640</v>
-          </cell>
-          <cell r="E175">
-            <v>9771792</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="B176" t="str">
-            <v>UL16</v>
-          </cell>
-          <cell r="C176">
-            <v>9980688</v>
-          </cell>
-          <cell r="D176">
-            <v>10865680</v>
-          </cell>
-          <cell r="E176">
-            <v>13258128</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="B177" t="str">
-            <v>UL64</v>
-          </cell>
-          <cell r="C177">
-            <v>8970000</v>
-          </cell>
-          <cell r="D177">
-            <v>9118992</v>
-          </cell>
-          <cell r="E177">
-            <v>12649616</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="B178" t="str">
-            <v>UL64 + SIMD2</v>
-          </cell>
-          <cell r="C178">
-            <v>7087888</v>
-          </cell>
-          <cell r="D178">
-            <v>7294352</v>
-          </cell>
-          <cell r="E178">
-            <v>12857716</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="B179" t="str">
-            <v>UL64 + SIMD4</v>
-          </cell>
-          <cell r="C179">
-            <v>6567696</v>
-          </cell>
-          <cell r="D179">
-            <v>6317200</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="B180" t="str">
-            <v>UL64 + SIMD8</v>
-          </cell>
-          <cell r="C180">
-            <v>7730448</v>
-          </cell>
-          <cell r="D180">
-            <v>6031376</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="B181" t="str">
-            <v>UL64 + SIMD16</v>
-          </cell>
-          <cell r="D181">
-            <v>6331664</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="B182" t="str">
-            <v>UL64+SIMD2+CU3</v>
-          </cell>
-          <cell r="C182">
-            <v>18067216</v>
-          </cell>
-          <cell r="D182">
-            <v>18559120</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="B183" t="str">
-            <v>UL64+SIMD2 +CU4</v>
-          </cell>
-          <cell r="C183">
-            <v>23030288</v>
-          </cell>
-          <cell r="D183">
-            <v>23859728</v>
-          </cell>
-        </row>
-        <row r="184">
-          <cell r="B184" t="str">
-            <v>UL64+SIMD4+CU3</v>
-          </cell>
-          <cell r="C184">
-            <v>16506640</v>
-          </cell>
-          <cell r="D184">
-            <v>15627664</v>
-          </cell>
-        </row>
-        <row r="185">
-          <cell r="B185" t="str">
-            <v>UL64+SIMD8+CU2</v>
-          </cell>
-          <cell r="D185">
-            <v>10731536</v>
-          </cell>
-        </row>
-        <row r="190">
-          <cell r="C190" t="str">
-            <v>float16</v>
-          </cell>
-          <cell r="D190" t="str">
-            <v>float</v>
-          </cell>
-          <cell r="E190" t="str">
-            <v>double</v>
-          </cell>
-        </row>
-        <row r="191">
-          <cell r="B191" t="str">
-            <v>Baseline</v>
-          </cell>
-          <cell r="C191">
-            <v>752</v>
-          </cell>
-          <cell r="D191">
-            <v>762</v>
-          </cell>
-          <cell r="E191">
-            <v>940</v>
-          </cell>
-        </row>
-        <row r="192">
-          <cell r="B192" t="str">
-            <v>SIMD4</v>
-          </cell>
-          <cell r="C192">
-            <v>540</v>
-          </cell>
-          <cell r="D192">
-            <v>573</v>
-          </cell>
-          <cell r="E192">
-            <v>807</v>
-          </cell>
-        </row>
-        <row r="193">
-          <cell r="B193" t="str">
-            <v>UL16</v>
-          </cell>
-          <cell r="C193">
-            <v>768</v>
-          </cell>
-          <cell r="D193">
-            <v>793</v>
-          </cell>
-          <cell r="E193">
-            <v>1028</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="B194" t="str">
-            <v>UL64</v>
-          </cell>
-          <cell r="C194">
-            <v>766</v>
-          </cell>
-          <cell r="D194">
-            <v>744</v>
-          </cell>
-          <cell r="E194">
-            <v>1107</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="B195" t="str">
-            <v>UL64 + SIMD2</v>
-          </cell>
-          <cell r="C195">
-            <v>712</v>
-          </cell>
-          <cell r="D195">
-            <v>699</v>
-          </cell>
-          <cell r="E195">
-            <v>1322</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="B196" t="str">
-            <v>UL64 + SIMD4</v>
-          </cell>
-          <cell r="C196">
-            <v>791</v>
-          </cell>
-          <cell r="D196">
-            <v>753</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="B197" t="str">
-            <v>UL64 + SIMD8</v>
-          </cell>
-          <cell r="C197">
-            <v>1106</v>
-          </cell>
-          <cell r="D197">
-            <v>1005</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="B198" t="str">
-            <v>UL64 + SIMD16</v>
-          </cell>
-          <cell r="D198">
-            <v>1561</v>
-          </cell>
-        </row>
-        <row r="199">
-          <cell r="B199" t="str">
-            <v>UL64+SIMD2+CU3</v>
-          </cell>
-          <cell r="C199">
-            <v>1585</v>
-          </cell>
-          <cell r="D199">
-            <v>1677</v>
-          </cell>
-        </row>
-        <row r="200">
-          <cell r="B200" t="str">
-            <v>UL64+SIMD2 +CU4</v>
-          </cell>
-          <cell r="C200">
-            <v>2017</v>
-          </cell>
-          <cell r="D200">
-            <v>2148</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="B201" t="str">
-            <v>UL64+SIMD4+CU3</v>
-          </cell>
-          <cell r="C201">
-            <v>1822</v>
-          </cell>
-          <cell r="D201">
-            <v>1839</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="B202" t="str">
-            <v>UL64+SIMD8+CU2</v>
-          </cell>
-          <cell r="D202">
-            <v>1818</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1844,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2465,11 +1844,11 @@
         <v>62.12</v>
       </c>
       <c r="K16" s="17">
-        <f>MMULT(I16,J16)*1000</f>
+        <f t="shared" ref="K16:K22" si="2">MMULT(I16,J16)*1000</f>
         <v>16306500</v>
       </c>
       <c r="L16" s="23">
-        <f>4294.9673/J16</f>
+        <f t="shared" ref="L16:L22" si="3">4294.9673/J16</f>
         <v>69.139847070186747</v>
       </c>
     </row>
@@ -2505,11 +1884,11 @@
         <v>32.390999999999998</v>
       </c>
       <c r="K17" s="17">
-        <f>MMULT(I17,J17)*1000</f>
+        <f t="shared" si="2"/>
         <v>8043765.0000215936</v>
       </c>
       <c r="L17" s="23">
-        <f>4294.9673/J17</f>
+        <f t="shared" si="3"/>
         <v>132.59755178907722</v>
       </c>
     </row>
@@ -2545,11 +1924,11 @@
         <v>19.164000000000001</v>
       </c>
       <c r="K18" s="17">
-        <f>MMULT(I18,J18)*1000</f>
+        <f t="shared" si="2"/>
         <v>4455630</v>
       </c>
       <c r="L18" s="23">
-        <f>4294.9673/J18</f>
+        <f t="shared" si="3"/>
         <v>224.11643185138803</v>
       </c>
     </row>
@@ -2585,11 +1964,11 @@
         <v>35.664999999999999</v>
       </c>
       <c r="K19" s="17">
-        <f>MMULT(I19,J19)*1000</f>
+        <f t="shared" si="2"/>
         <v>8500158.3333571106</v>
       </c>
       <c r="L19" s="23">
-        <f>4294.9673/J19</f>
+        <f t="shared" si="3"/>
         <v>120.42527127435862</v>
       </c>
     </row>
@@ -2623,11 +2002,11 @@
         <v>815.221</v>
       </c>
       <c r="K20" s="17">
-        <f>MMULT(I20,J20)*1000</f>
+        <f t="shared" si="2"/>
         <v>269022930</v>
       </c>
       <c r="L20" s="23">
-        <f>4294.9673/J20</f>
+        <f t="shared" si="3"/>
         <v>5.2684698995732449</v>
       </c>
     </row>
@@ -2661,11 +2040,11 @@
         <v>111.19499999999999</v>
       </c>
       <c r="K21" s="17">
-        <f>MMULT(I21,J21)*1000</f>
+        <f t="shared" si="2"/>
         <v>33705984.375</v>
       </c>
       <c r="L21" s="23">
-        <f>4294.9673/J21</f>
+        <f t="shared" si="3"/>
         <v>38.625543414721889</v>
       </c>
     </row>
@@ -2699,11 +2078,11 @@
         <v>218.173</v>
       </c>
       <c r="K22" s="17">
-        <f>MMULT(I22,J22)*1000</f>
+        <f t="shared" si="2"/>
         <v>67270008.333260596</v>
       </c>
       <c r="L22" s="23">
-        <f>4294.9673/J22</f>
+        <f t="shared" si="3"/>
         <v>19.68606243669015</v>
       </c>
     </row>
@@ -2737,11 +2116,11 @@
         <v>170.22900000000001</v>
       </c>
       <c r="K23" s="17">
-        <f t="shared" ref="K23:K27" si="2">MMULT(I23,J23)*1000</f>
+        <f t="shared" ref="K23:K27" si="4">MMULT(I23,J23)*1000</f>
         <v>36705628.125</v>
       </c>
       <c r="L23" s="23">
-        <f t="shared" ref="L23:L27" si="3">4294.9673/J23</f>
+        <f t="shared" ref="L23:L27" si="5">4294.9673/J23</f>
         <v>25.23052652603258</v>
       </c>
     </row>
@@ -2775,11 +2154,11 @@
         <v>36.573999999999998</v>
       </c>
       <c r="K24" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9417805</v>
       </c>
       <c r="L24" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>117.43225515393451</v>
       </c>
     </row>
@@ -2813,11 +2192,11 @@
         <v>18.157</v>
       </c>
       <c r="K25" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4369028.125</v>
       </c>
       <c r="L25" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>236.54608690863029</v>
       </c>
     </row>
@@ -2851,11 +2230,11 @@
         <v>72.494</v>
       </c>
       <c r="K26" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16915266.666714996</v>
       </c>
       <c r="L26" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>59.245831379148626</v>
       </c>
     </row>
@@ -2889,11 +2268,11 @@
         <v>37.93</v>
       </c>
       <c r="K27" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8534250</v>
       </c>
       <c r="L27" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>113.23404429211706</v>
       </c>
     </row>
@@ -2902,7 +2281,7 @@
         <v>148</v>
       </c>
       <c r="B31" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="1"/>
@@ -3015,11 +2394,11 @@
         <v>10522.106</v>
       </c>
       <c r="K34" s="17">
-        <f t="shared" ref="K34:K35" si="4">MMULT(I34,J34)*1000</f>
+        <f t="shared" ref="K34:K35" si="6">MMULT(I34,J34)*1000</f>
         <v>3726579208.3368406</v>
       </c>
       <c r="L34" s="9">
-        <f t="shared" ref="L34:L35" si="5">4294.9673/J34</f>
+        <f t="shared" ref="L34:L35" si="7">4294.9673/J34</f>
         <v>0.40818513898263337</v>
       </c>
     </row>
@@ -3055,153 +2434,245 @@
         <v>10521.141</v>
       </c>
       <c r="K35" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3130039447.5</v>
       </c>
       <c r="L35" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.40822257776033993</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="9"/>
-    </row>
-    <row r="37" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="9"/>
-    </row>
-    <row r="38" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A38" s="1"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="9"/>
-    </row>
-    <row r="39" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A39" s="1"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="9"/>
-    </row>
-    <row r="40" spans="1:12" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="1">
+        <v>59428</v>
+      </c>
+      <c r="D36" s="8">
+        <v>75710</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I36" s="16">
+        <v>285</v>
+      </c>
+      <c r="J36" s="1">
+        <v>7542.326</v>
+      </c>
+      <c r="K36" s="17">
+        <f>MMULT(I36,J36)*1000</f>
+        <v>2149562910</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="1">
+        <v>60232</v>
+      </c>
+      <c r="D37" s="8">
+        <v>76305</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I37" s="16">
+        <v>211.11111111100001</v>
+      </c>
+      <c r="J37" s="1">
+        <v>10184.028</v>
+      </c>
+      <c r="K37" s="17">
+        <f>MMULT(I37,J37)*1000</f>
+        <v>2149961466.6655354</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="1">
+        <v>65521</v>
+      </c>
+      <c r="D38" s="8">
+        <v>82226</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I38" s="16">
+        <v>275</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1960.117</v>
+      </c>
+      <c r="K38" s="17">
+        <f t="shared" ref="K38:K41" si="8">MMULT(I38,J38)*1000</f>
+        <v>539032175</v>
+      </c>
+      <c r="L38" s="9">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" s="1">
+        <v>70218</v>
+      </c>
+      <c r="D39" s="8">
+        <v>87782</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I39" s="16">
+        <v>281.25</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1099.5350000000001</v>
+      </c>
+      <c r="K39" s="17">
+        <f t="shared" si="8"/>
+        <v>309244218.75</v>
+      </c>
+      <c r="L39" s="9">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="27" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="17"/>
-    </row>
-    <row r="41" spans="1:12" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="A41" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J41" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="K41" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
-      <c r="A42" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="1">
-        <v>61472</v>
-      </c>
-      <c r="D42" s="8">
-        <v>78098</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I42" s="16">
-        <v>335</v>
-      </c>
-      <c r="J42" s="1">
-        <v>10537.268</v>
-      </c>
-      <c r="K42" s="17">
-        <f>MMULT(I42,J42)*1000</f>
-        <v>3529984780</v>
-      </c>
-      <c r="L42" s="9">
-        <f>4294.9673/J42</f>
-        <v>0.40759780428854997</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C40" s="3">
+        <v>84426</v>
+      </c>
+      <c r="D40" s="28">
+        <v>99964</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="2">
+        <v>272.5</v>
+      </c>
+      <c r="J40" s="3">
+        <v>571.40099999999995</v>
+      </c>
+      <c r="K40" s="4">
+        <f t="shared" si="8"/>
+        <v>155706772.5</v>
+      </c>
+      <c r="L40" s="29">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="1">
+        <v>126763</v>
+      </c>
+      <c r="D41" s="8">
+        <v>125837</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I41" s="16">
+        <v>215</v>
+      </c>
+      <c r="J41" s="1">
+        <v>776.87</v>
+      </c>
+      <c r="K41" s="17">
+        <f t="shared" si="8"/>
+        <v>167027050</v>
+      </c>
+      <c r="L41" s="9">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="9"/>
     </row>
     <row r="43" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
@@ -3231,75 +2702,304 @@
       <c r="K44" s="17"/>
       <c r="L44" s="9"/>
     </row>
-    <row r="45" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A45" s="1"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+    <row r="45" spans="1:12" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="3">
+        <v>6</v>
+      </c>
       <c r="I45" s="16"/>
       <c r="J45" s="1"/>
       <c r="K45" s="17"/>
-      <c r="L45" s="9"/>
-    </row>
-    <row r="46" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A46" s="1"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="9"/>
-    </row>
-    <row r="47" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A47" s="1"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="9"/>
-    </row>
-    <row r="48" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A48" s="1"/>
+    </row>
+    <row r="46" spans="1:12" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.15">
+      <c r="A46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A47" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="1">
+        <v>61472</v>
+      </c>
+      <c r="D47" s="8">
+        <v>78098</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I47" s="16">
+        <v>335</v>
+      </c>
+      <c r="J47" s="1">
+        <v>10537.268</v>
+      </c>
+      <c r="K47" s="17">
+        <f>MMULT(I47,J47)*1000</f>
+        <v>3529984780</v>
+      </c>
+      <c r="L47" s="9">
+        <f>4294.9673/J47</f>
+        <v>0.40759780428854997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="B48" s="12"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="9"/>
-    </row>
-    <row r="49" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
-      <c r="A49" s="1"/>
+      <c r="C48" s="1">
+        <v>61514</v>
+      </c>
+      <c r="D48" s="8">
+        <v>78059</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I48" s="16">
+        <v>343.75</v>
+      </c>
+      <c r="J48" s="1">
+        <v>6274.62</v>
+      </c>
+      <c r="K48" s="17">
+        <f t="shared" ref="K48:K52" si="9">MMULT(I48,J48)*1000</f>
+        <v>2156900625</v>
+      </c>
+      <c r="L48" s="23">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="B49" s="12"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="9"/>
+      <c r="C49" s="1">
+        <v>64919</v>
+      </c>
+      <c r="D49" s="8">
+        <v>82845</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I49" s="16">
+        <v>295</v>
+      </c>
+      <c r="J49" s="1">
+        <v>1864.5619999999999</v>
+      </c>
+      <c r="K49" s="17">
+        <f t="shared" si="9"/>
+        <v>550045789.99999988</v>
+      </c>
+      <c r="L49" s="23">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="30"/>
+      <c r="C50" s="3">
+        <v>68002</v>
+      </c>
+      <c r="D50" s="28">
+        <v>87147</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I50" s="2">
+        <v>287.5</v>
+      </c>
+      <c r="J50" s="3">
+        <v>1153.347</v>
+      </c>
+      <c r="K50" s="4">
+        <f t="shared" si="9"/>
+        <v>331587262.5</v>
+      </c>
+      <c r="L50" s="31">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" s="12"/>
+      <c r="C51" s="1">
+        <v>76004</v>
+      </c>
+      <c r="D51" s="8">
+        <v>95937</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I51" s="16">
+        <v>279.17</v>
+      </c>
+      <c r="J51" s="1">
+        <v>39920.902000000002</v>
+      </c>
+      <c r="K51" s="17">
+        <f t="shared" si="9"/>
+        <v>11144718211.34</v>
+      </c>
+      <c r="L51" s="23">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="1">
+        <v>100146</v>
+      </c>
+      <c r="D52" s="8">
+        <v>115336</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I52" s="16">
+        <v>227.5</v>
+      </c>
+      <c r="J52" s="1">
+        <v>48103.580999999998</v>
+      </c>
+      <c r="K52" s="17">
+        <f t="shared" si="9"/>
+        <v>10943564677.5</v>
+      </c>
+      <c r="L52" s="23">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A53" s="1"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:12" s="10" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A54" s="1"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>